<commit_message>
Change resnet # filter multiple from 12 back to 16. Add checkpoints with multiple=16 filters.
</commit_message>
<xml_diff>
--- a/cifar10_resnet_accuracy.xlsx
+++ b/cifar10_resnet_accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weier Wan\Dropbox\cs231n\cifar10_resnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E619BD25-38DE-435A-A1E3-5568D3833747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E26433D-FDB3-45D7-861E-214ECE03CBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="5025" windowWidth="29040" windowHeight="15840" xr2:uid="{29F9E3F9-6959-4C90-BC3C-99386578FCBD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>None</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>3b (v2)</t>
+  </si>
+  <si>
+    <t>20% (excl input)</t>
+  </si>
+  <si>
+    <t>16filter_3b</t>
+  </si>
+  <si>
+    <t>0.15 (excl input)</t>
+  </si>
+  <si>
+    <t>0.2 (excl input)</t>
+  </si>
+  <si>
+    <t>15%(excl input)</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1707,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2104,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C667BF4-9686-42EC-9F3B-A0C70169C51C}">
-  <dimension ref="A2:L34"/>
+  <dimension ref="A2:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,198 +2482,309 @@
         <v>0.7833</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>0.86119999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="E23">
+        <v>0.82950000000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.78320000000000001</v>
+      </c>
+    </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>0</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>0.85829999999999995</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>0.59930000000000005</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>0.188</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>0.1108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25">
-        <v>0.05</v>
-      </c>
-      <c r="C25">
-        <v>0.8528</v>
-      </c>
-      <c r="D25">
-        <v>0.82079999999999997</v>
-      </c>
-      <c r="E25">
-        <v>0.71060000000000001</v>
-      </c>
-      <c r="F25">
-        <v>0.48159999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C26">
-        <v>0.84940000000000004</v>
+        <v>0.8528</v>
       </c>
       <c r="D26">
-        <v>0.83699999999999997</v>
+        <v>0.82079999999999997</v>
       </c>
       <c r="E26">
-        <v>0.78779999999999994</v>
+        <v>0.71060000000000001</v>
       </c>
       <c r="F26">
-        <v>0.67479999999999996</v>
+        <v>0.48159999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C27">
-        <v>0.8518</v>
+        <v>0.84940000000000004</v>
       </c>
       <c r="D27">
-        <v>0.84150000000000003</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="E27">
-        <v>0.81589999999999996</v>
+        <v>0.78779999999999994</v>
       </c>
       <c r="F27">
-        <v>0.75680000000000003</v>
+        <v>0.67479999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C28">
-        <v>0.84440000000000004</v>
+        <v>0.8518</v>
       </c>
       <c r="D28">
-        <v>0.84019999999999995</v>
+        <v>0.84150000000000003</v>
       </c>
       <c r="E28">
-        <v>0.81659999999999999</v>
+        <v>0.81589999999999996</v>
       </c>
       <c r="F28">
-        <v>0.7863</v>
+        <v>0.75680000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="C29">
-        <v>0.83009999999999995</v>
+        <v>0.84440000000000004</v>
       </c>
       <c r="D29">
-        <v>0.82630000000000003</v>
+        <v>0.84019999999999995</v>
       </c>
       <c r="E29">
-        <v>0.81240000000000001</v>
+        <v>0.81659999999999999</v>
       </c>
       <c r="F29">
-        <v>0.79310000000000003</v>
+        <v>0.7863</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30">
+        <v>0.25</v>
+      </c>
+      <c r="C30">
+        <v>0.83009999999999995</v>
+      </c>
+      <c r="D30">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="E30">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="F30">
+        <v>0.79310000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31">
         <v>0.3</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>0.82089999999999996</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.81659999999999999</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>0.80669999999999997</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>0.79430000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>0.8669</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>0.55189999999999995</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>0.16850000000000001</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>0.1106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33">
-        <v>0.15</v>
-      </c>
-      <c r="C33">
-        <v>0.8619</v>
-      </c>
-      <c r="D33">
-        <v>0.85309999999999997</v>
-      </c>
-      <c r="E33">
-        <v>0.82830000000000004</v>
-      </c>
-      <c r="F33">
-        <v>0.76900000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34">
+        <v>0.15</v>
+      </c>
+      <c r="C34">
+        <v>0.8619</v>
+      </c>
+      <c r="D34">
+        <v>0.85309999999999997</v>
+      </c>
+      <c r="E34">
+        <v>0.82830000000000004</v>
+      </c>
+      <c r="F34">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35">
         <v>0.2</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>0.84909999999999997</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>0.84819999999999995</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>0.83050000000000002</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>0.79500000000000004</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>0.15</v>
+      </c>
+      <c r="C37">
+        <v>0.86529999999999996</v>
+      </c>
+      <c r="D37">
+        <v>0.86329999999999996</v>
+      </c>
+      <c r="E37">
+        <v>0.84089999999999998</v>
+      </c>
+      <c r="F37">
+        <v>0.79849999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38">
+        <v>0.2</v>
+      </c>
+      <c r="C38">
+        <v>0.86380000000000001</v>
+      </c>
+      <c r="D38">
+        <v>0.8579</v>
+      </c>
+      <c r="E38">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="F38">
+        <v>0.82320000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="D39">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="E39">
+        <v>0.86150000000000004</v>
+      </c>
+      <c r="F39">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>0.87819999999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.87549999999999994</v>
+      </c>
+      <c r="E40">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="F40">
+        <v>0.83560000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A16:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bug fixes and add input segmenting to conv/dense numpy implementation
</commit_message>
<xml_diff>
--- a/cifar10_resnet_accuracy.xlsx
+++ b/cifar10_resnet_accuracy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weier Wan\Dropbox\cs231n\cifar10_resnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E26433D-FDB3-45D7-861E-214ECE03CBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04D154-AFF5-4A87-9B9B-4805F3F16189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="5025" windowWidth="29040" windowHeight="15840" xr2:uid="{29F9E3F9-6959-4C90-BC3C-99386578FCBD}"/>
+    <workbookView xWindow="32175" yWindow="7770" windowWidth="21600" windowHeight="11385" xr2:uid="{29F9E3F9-6959-4C90-BC3C-99386578FCBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>None</t>
   </si>
@@ -50,19 +50,10 @@
     <t>baseline</t>
   </si>
   <si>
-    <t>12filters</t>
-  </si>
-  <si>
     <t>4b （excl input)</t>
   </si>
   <si>
-    <t>3b（excl input)</t>
-  </si>
-  <si>
     <t>2b（excl input)</t>
-  </si>
-  <si>
-    <t>3b (0.95)</t>
   </si>
   <si>
     <t>3b (0.9)</t>
@@ -84,6 +75,24 @@
   </si>
   <si>
     <t>15%(excl input)</t>
+  </si>
+  <si>
+    <t>12 filters</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>3b (excl input)</t>
+  </si>
+  <si>
+    <t>0 (excl input)</t>
+  </si>
+  <si>
+    <t>16filter_3b (excl input)</t>
+  </si>
+  <si>
+    <t>24filter_3b</t>
   </si>
 </sst>
 </file>
@@ -183,93 +192,6 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$15:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$16:$F$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.85529999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1449</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1082</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-9F05-4001-BFC8-812751BA309C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -330,21 +252,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$F$17</c:f>
+              <c:f>Sheet1!$C$38:$F$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.85550000000000004</c:v>
+                  <c:v>0.87439999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81679999999999997</c:v>
+                  <c:v>0.85319999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68830000000000002</c:v>
+                  <c:v>0.77059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46689999999999998</c:v>
+                  <c:v>0.58530000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -417,21 +339,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$F$18</c:f>
+              <c:f>Sheet1!$C$39:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.85529999999999995</c:v>
+                  <c:v>0.87080000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84019999999999995</c:v>
+                  <c:v>0.86140000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79279999999999995</c:v>
+                  <c:v>0.82779999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69179999999999997</c:v>
+                  <c:v>0.74650000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -504,21 +426,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$F$19</c:f>
+              <c:f>Sheet1!$C$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.84319999999999995</c:v>
+                  <c:v>0.86529999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83489999999999998</c:v>
+                  <c:v>0.86329999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81020000000000003</c:v>
+                  <c:v>0.84089999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75600000000000001</c:v>
+                  <c:v>0.79849999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -591,21 +513,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$F$20</c:f>
+              <c:f>Sheet1!$C$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.83899999999999997</c:v>
+                  <c:v>0.86380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83509999999999995</c:v>
+                  <c:v>0.8579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81720000000000004</c:v>
+                  <c:v>0.84750000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78039999999999998</c:v>
+                  <c:v>0.82320000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,21 +600,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$F$21</c:f>
+              <c:f>Sheet1!$C$42:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.83160000000000001</c:v>
+                  <c:v>0.85440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82730000000000004</c:v>
+                  <c:v>0.85470000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8135</c:v>
+                  <c:v>0.84440000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79269999999999996</c:v>
+                  <c:v>0.82630000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -771,21 +693,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$F$22</c:f>
+              <c:f>Sheet1!$C$43:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8236</c:v>
+                  <c:v>0.84770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8196</c:v>
+                  <c:v>0.8468</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.80930000000000002</c:v>
+                  <c:v>0.83550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7833</c:v>
+                  <c:v>0.82320000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -807,6 +729,117 @@
         </c:dLbls>
         <c:axId val="2022242015"/>
         <c:axId val="2015188959"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0%</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$15:$F$15</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.05</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$37:$F$37</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0.87039999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.6673</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.24340000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.1222</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-9F05-4001-BFC8-812751BA309C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2022242015"/>
@@ -1139,7 +1172,362 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>accuracy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$K$2,Sheet1!$K$3,Sheet1!$A$7,Sheet1!$A$16)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12 filters</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3b (excl input)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$L$2,Sheet1!$L$3,Sheet1!$C$8,Sheet1!$C$16)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90539999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89080000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88139999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85529999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7122-4E62-9471-80FA86FCDC55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="192420351"/>
+        <c:axId val="446647615"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="192420351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446647615"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="446647615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.84000000000000008"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192420351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1676,6 +2064,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1819,6 +2710,42 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>477638</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19B5B9CC-4270-4F2C-9639-52C88222241F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2119,10 +3046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C667BF4-9686-42EC-9F3B-A0C70169C51C}">
-  <dimension ref="A2:L40"/>
+  <dimension ref="A2:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,7 +3086,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2174,7 +3101,7 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>0.89080000000000004</v>
@@ -2227,7 +3154,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -2307,7 +3234,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -2356,7 +3283,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2485,7 +3412,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>0.86119999999999997</v>
@@ -2503,7 +3430,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" s="2">
         <v>0.85750000000000004</v>
@@ -2520,7 +3447,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2648,7 +3575,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -2704,87 +3631,378 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37">
-        <v>0.15</v>
+        <v>10</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>0.86529999999999996</v>
+        <v>0.87039999999999995</v>
       </c>
       <c r="D37">
-        <v>0.86329999999999996</v>
+        <v>0.6673</v>
       </c>
       <c r="E37">
-        <v>0.84089999999999998</v>
+        <v>0.24340000000000001</v>
       </c>
       <c r="F37">
-        <v>0.79849999999999999</v>
+        <v>0.1222</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38">
-        <v>0.2</v>
+      <c r="B38" s="3">
+        <v>0.05</v>
       </c>
       <c r="C38">
-        <v>0.86380000000000001</v>
+        <v>0.87439999999999996</v>
       </c>
       <c r="D38">
-        <v>0.8579</v>
+        <v>0.85319999999999996</v>
       </c>
       <c r="E38">
-        <v>0.84750000000000003</v>
+        <v>0.77059999999999995</v>
       </c>
       <c r="F38">
-        <v>0.82320000000000004</v>
+        <v>0.58530000000000004</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" t="s">
-        <v>14</v>
+      <c r="B39" s="3">
+        <v>0.1</v>
       </c>
       <c r="C39">
-        <v>0.88219999999999998</v>
+        <v>0.87080000000000002</v>
       </c>
       <c r="D39">
-        <v>0.87680000000000002</v>
+        <v>0.86140000000000005</v>
       </c>
       <c r="E39">
-        <v>0.86150000000000004</v>
+        <v>0.82779999999999998</v>
       </c>
       <c r="F39">
-        <v>0.82499999999999996</v>
+        <v>0.74650000000000005</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" t="s">
-        <v>15</v>
+      <c r="B40" s="3">
+        <v>0.15</v>
       </c>
       <c r="C40">
+        <v>0.86529999999999996</v>
+      </c>
+      <c r="D40">
+        <v>0.86329999999999996</v>
+      </c>
+      <c r="E40">
+        <v>0.84089999999999998</v>
+      </c>
+      <c r="F40">
+        <v>0.79849999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C41">
+        <v>0.86380000000000001</v>
+      </c>
+      <c r="D41">
+        <v>0.8579</v>
+      </c>
+      <c r="E41">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="F41">
+        <v>0.82320000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C42">
+        <v>0.85440000000000005</v>
+      </c>
+      <c r="D42">
+        <v>0.85470000000000002</v>
+      </c>
+      <c r="E42">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F42">
+        <v>0.82630000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C43">
+        <v>0.84770000000000001</v>
+      </c>
+      <c r="D43">
+        <v>0.8468</v>
+      </c>
+      <c r="E43">
+        <v>0.83550000000000002</v>
+      </c>
+      <c r="F43">
+        <v>0.82320000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="D44">
+        <v>0.69330000000000003</v>
+      </c>
+      <c r="E44">
+        <v>0.26619999999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.1217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="D45">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="E45">
+        <v>0.86150000000000004</v>
+      </c>
+      <c r="F45">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
         <v>0.87819999999999998</v>
       </c>
-      <c r="D40">
+      <c r="D46">
         <v>0.87549999999999994</v>
       </c>
-      <c r="E40">
+      <c r="E46">
         <v>0.86250000000000004</v>
       </c>
-      <c r="F40">
+      <c r="F46">
         <v>0.83560000000000001</v>
       </c>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0.89659999999999995</v>
+      </c>
+      <c r="D47">
+        <v>0.61750000000000005</v>
+      </c>
+      <c r="E47">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="F47">
+        <v>0.1103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C48">
+        <v>0.89470000000000005</v>
+      </c>
+      <c r="D48">
+        <v>0.87470000000000003</v>
+      </c>
+      <c r="E48">
+        <v>0.7873</v>
+      </c>
+      <c r="F48">
+        <v>0.59219999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C49">
+        <v>0.8921</v>
+      </c>
+      <c r="D49">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="E49">
+        <v>0.84819999999999995</v>
+      </c>
+      <c r="F49">
+        <v>0.76380000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C50">
+        <v>0.8911</v>
+      </c>
+      <c r="D50">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="E50">
+        <v>0.86880000000000002</v>
+      </c>
+      <c r="F50">
+        <v>0.82169999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C51">
+        <v>0.88039999999999996</v>
+      </c>
+      <c r="D51">
+        <v>0.87629999999999997</v>
+      </c>
+      <c r="E51">
+        <v>0.86209999999999998</v>
+      </c>
+      <c r="F51">
+        <v>0.83379999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C52">
+        <v>0.87390000000000001</v>
+      </c>
+      <c r="D52">
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="E52">
+        <v>0.85970000000000002</v>
+      </c>
+      <c r="F52">
+        <v>0.84389999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C53">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="D53">
+        <v>0.86319999999999997</v>
+      </c>
+      <c r="E53">
+        <v>0.85629999999999995</v>
+      </c>
+      <c r="F53">
+        <v>0.84250000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C55">
+        <v>0.89219999999999999</v>
+      </c>
+      <c r="D55">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="E55">
+        <v>0.86990000000000001</v>
+      </c>
+      <c r="F55">
+        <v>0.84519999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C56">
+        <v>0.88739999999999997</v>
+      </c>
+      <c r="D56">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="E56">
+        <v>0.87519999999999998</v>
+      </c>
+      <c r="F56">
+        <v>0.8619</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C57">
+        <v>0.8851</v>
+      </c>
+      <c r="D57">
+        <v>0.88229999999999997</v>
+      </c>
+      <c r="E57">
+        <v>0.87649999999999995</v>
+      </c>
+      <c r="F57">
+        <v>0.85719999999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A37:A40"/>
+  <mergeCells count="8">
+    <mergeCell ref="A47:A53"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A16:A24"/>
+    <mergeCell ref="A37:A46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>